<commit_message>
Update convertExcel, and include contentful-management to allow for parsing of excel, and upload to Contentful
Update app to crawl excel sheets more effectively, upload locales in batches, and avoid API rate limit by using setTimeout

Handle right justified right justified text for locales that read right to left
</commit_message>
<xml_diff>
--- a/excelDocs/testSheet.xlsx
+++ b/excelDocs/testSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-34000" yWindow="1760" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="2060" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,51 +71,29 @@
     <t>troubleshootingInstructions</t>
   </si>
   <si>
-    <t>DK1s4wpVkcKOcuSYwkai4</t>
-  </si>
-  <si>
-    <t>If you followed the connection steps, but you're still having trouble connecting your device, you may need to reset your device through a Z-Wave exclusion. Note: The Z-Wave exclusion will still reset your device if it has never been connected before or was previously connected elsewhere.
-1. Put the Hub into exclusion mode
-        a. Tap the back button until you reach the Home screen and tap the Hub 
-        b. Tap the three dots in the top right
-        c. Tap Z-Wave exclusion
-2. Press up and release the toggle switch
-After your device has been successfully excluded, follow the steps below to connect your device to the Hub. 
-1. Return to the device connection screen
-        a. Tap the back button until you reach the Home screen
-        b. Tap Add device
-        c. Select a category to find your device, or search for the device in the search bar
-2. Press up and release the toggle switch</t>
-  </si>
-  <si>
     <t>In-Wall Smart Outlet (Z-Wave)</t>
   </si>
   <si>
     <t>[GE 12721]</t>
   </si>
   <si>
-    <t>5as7fDSCeQsycUWkYo2kKS</t>
-  </si>
-  <si>
-    <t>If you followed the connection steps, but you're still having trouble connecting your device, you may need to reset your device through a Z-Wave exclusion. Note: The Z-Wave exclusion will still reset your device if it has never been connected before or was previously connected elsewhere.
-1. Put the Hub into exclusion mode
-        a. Tap the back button until you reach the Home screen and tap the Hub 
-        b. Tap the three dots in the top right
-        c. Tap Z-Wave exclusion
-2. Push the button on the face of the outlet once
-After your device has been successfully excluded, follow the steps below to connect your device to the Hub. 
-1. Return to the device connection screen
-        a. Tap the back button until you reach the Home screen
-        b. Tap Add device
-        c. Select a category to find your device, or search for the device in the search bar
-2. Push the button on the face of the outlet once</t>
+    <t>TTTTEEESSSTTTT</t>
+  </si>
+  <si>
+    <t>aTTTTEEESSSTTTT</t>
+  </si>
+  <si>
+    <t>1POcF3SaAkAoSWugQU22WK</t>
+  </si>
+  <si>
+    <t>5iDDJZZYicYAkCQk6U6OGM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -135,6 +113,11 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF536171"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="2">
@@ -157,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -167,6 +150,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,11 +430,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -478,7 +465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -498,21 +485,21 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
@@ -523,11 +510,11 @@
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
-        <v>18</v>
+      <c r="G3" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>